<commit_message>
Final update to lab 4 with related source code files
</commit_message>
<xml_diff>
--- a/labcode/sample student marks.xlsx
+++ b/labcode/sample student marks.xlsx
@@ -5,27 +5,35 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\workshops\javascript\shopee appscript\labcode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{534237CC-B629-4C56-AF33-49B85187E670}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{153D4C85-74CB-416E-8783-1C65D8D4F30C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25710" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Students" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>English</t>
   </si>
@@ -67,21 +75,6 @@
   </si>
   <si>
     <t>Student10</t>
-  </si>
-  <si>
-    <t>Student11</t>
-  </si>
-  <si>
-    <t>Student12</t>
-  </si>
-  <si>
-    <t>Student13</t>
-  </si>
-  <si>
-    <t>Student14</t>
-  </si>
-  <si>
-    <t>Student15</t>
   </si>
   <si>
     <t>Student Name</t>
@@ -411,10 +404,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -424,7 +417,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -450,7 +443,7 @@
         <v>45</v>
       </c>
       <c r="D2" s="1">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E2" s="1">
         <v>78</v>
@@ -461,16 +454,16 @@
         <v>5</v>
       </c>
       <c r="B3" s="1">
-        <v>25</v>
+        <v>58</v>
       </c>
       <c r="C3" s="1">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="D3" s="1">
-        <v>34</v>
+        <v>85</v>
       </c>
       <c r="E3" s="1">
-        <v>90</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.45">
@@ -481,10 +474,10 @@
         <v>89</v>
       </c>
       <c r="C4" s="1">
-        <v>89</v>
+        <v>62</v>
       </c>
       <c r="D4" s="1">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="E4" s="1">
         <v>45</v>
@@ -501,10 +494,10 @@
         <v>24</v>
       </c>
       <c r="D5" s="1">
-        <v>97</v>
+        <v>55</v>
       </c>
       <c r="E5" s="1">
-        <v>23</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.45">
@@ -512,10 +505,10 @@
         <v>8</v>
       </c>
       <c r="B6" s="1">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="C6" s="1">
-        <v>34</v>
+        <v>54</v>
       </c>
       <c r="D6" s="1">
         <v>24</v>
@@ -583,10 +576,10 @@
         <v>97</v>
       </c>
       <c r="C10" s="1">
-        <v>87</v>
+        <v>69</v>
       </c>
       <c r="D10" s="1">
-        <v>78</v>
+        <v>57</v>
       </c>
       <c r="E10" s="1">
         <v>45</v>
@@ -597,101 +590,16 @@
         <v>13</v>
       </c>
       <c r="B11" s="1">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="C11" s="1">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="D11" s="1">
-        <v>24</v>
+        <v>65</v>
       </c>
       <c r="E11" s="1">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="1">
-        <v>98</v>
-      </c>
-      <c r="C12" s="1">
-        <v>74</v>
-      </c>
-      <c r="D12" s="1">
-        <v>53</v>
-      </c>
-      <c r="E12" s="1">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A13" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" s="1">
-        <v>34</v>
-      </c>
-      <c r="C13" s="1">
-        <v>37</v>
-      </c>
-      <c r="D13" s="1">
-        <v>89</v>
-      </c>
-      <c r="E13" s="1">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A14" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="1">
-        <v>23</v>
-      </c>
-      <c r="C14" s="1">
-        <v>47</v>
-      </c>
-      <c r="D14" s="1">
-        <v>14</v>
-      </c>
-      <c r="E14" s="1">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A15" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" s="1">
-        <v>89</v>
-      </c>
-      <c r="C15" s="1">
-        <v>23</v>
-      </c>
-      <c r="D15" s="1">
-        <v>15</v>
-      </c>
-      <c r="E15" s="1">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A16" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16" s="1">
-        <v>34</v>
-      </c>
-      <c r="C16" s="1">
-        <v>64</v>
-      </c>
-      <c r="D16" s="1">
-        <v>24</v>
-      </c>
-      <c r="E16" s="1">
-        <v>33</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>